<commit_message>
update experiment list files
</commit_message>
<xml_diff>
--- a/experiment_list_balanced_data_full.xlsx
+++ b/experiment_list_balanced_data_full.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\scFiLM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F1DE68-59B2-4228-94BA-6DF795514EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA156E6-1458-4632-841D-C03B16CFB453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>./data/feature_number/sciplex_hvg_500.h5ad</t>
-  </si>
-  <si>
     <t>hvg_500</t>
   </si>
   <si>
@@ -87,72 +84,33 @@
     <t>hvg_7500</t>
   </si>
   <si>
-    <t>./data/feature_number/sciplex_hvg_1000.h5ad</t>
-  </si>
-  <si>
-    <t>./data/feature_number/sciplex_hvg_2000.h5ad</t>
-  </si>
-  <si>
-    <t>./data/feature_number/sciplex_hvg_3500.h5ad</t>
-  </si>
-  <si>
-    <t>./data/feature_number/sciplex_hvg_5000.h5ad</t>
-  </si>
-  <si>
-    <t>./data/feature_number/sciplex_hvg_7500.h5ad</t>
-  </si>
-  <si>
     <t>feature_selection</t>
   </si>
   <si>
-    <t>./data/feature_selection/sciplex_rand.h5ad</t>
-  </si>
-  <si>
     <t>random_features</t>
   </si>
   <si>
-    <t>./data/feature_selection/sciplex_seurat.h5ad</t>
-  </si>
-  <si>
     <t>seurat</t>
   </si>
   <si>
     <t>seurat_v3</t>
   </si>
   <si>
-    <t>./data/feature_selection/sciplex_seurat_v3.h5ad</t>
-  </si>
-  <si>
     <t>cellranger</t>
   </si>
   <si>
-    <t>./data/feature_selection/sciplex_cellranger.h5ad</t>
-  </si>
-  <si>
     <t>normalization</t>
   </si>
   <si>
     <t>raw</t>
   </si>
   <si>
-    <t>./data/normalization/sciplex_raw_filt.h5ad</t>
-  </si>
-  <si>
     <t>CPM</t>
   </si>
   <si>
-    <t>./data/normalization/sciplex_cpm_filt.h5ad</t>
-  </si>
-  <si>
     <t>shifted_logarithm</t>
   </si>
   <si>
-    <t>./data/normalization/sciplex_shiftedlog_filt.h5ad</t>
-  </si>
-  <si>
-    <t>./data/normalization/sciplex_analyticpearson_filt.h5ad</t>
-  </si>
-  <si>
     <t>analytic_pearson</t>
   </si>
   <si>
@@ -364,6 +322,48 @@
   </si>
   <si>
     <t>./results_balanced_data/normalization/prnet_analyticpearson_norm_res.pkl</t>
+  </si>
+  <si>
+    <t>./data_balanced/feature_number/sciplex_hvg_500.h5ad</t>
+  </si>
+  <si>
+    <t>./data_balanced/feature_number/sciplex_hvg_1000.h5ad</t>
+  </si>
+  <si>
+    <t>./data_balanced/feature_number/sciplex_hvg_2000.h5ad</t>
+  </si>
+  <si>
+    <t>./data_balanced/feature_number/sciplex_hvg_3500.h5ad</t>
+  </si>
+  <si>
+    <t>./data_balanced/feature_number/sciplex_hvg_5000.h5ad</t>
+  </si>
+  <si>
+    <t>./data_balanced/feature_number/sciplex_hvg_7500.h5ad</t>
+  </si>
+  <si>
+    <t>./data_balanced/feature_selection/sciplex_rand.h5ad</t>
+  </si>
+  <si>
+    <t>./data_balanced/feature_selection/sciplex_seurat.h5ad</t>
+  </si>
+  <si>
+    <t>./data_balanced/feature_selection/sciplex_seurat_v3.h5ad</t>
+  </si>
+  <si>
+    <t>./data_balanced/feature_selection/sciplex_cellranger.h5ad</t>
+  </si>
+  <si>
+    <t>./data_balanced/normalization/sciplex_raw_filt.h5ad</t>
+  </si>
+  <si>
+    <t>./data_balanced/normalization/sciplex_cpm_filt.h5ad</t>
+  </si>
+  <si>
+    <t>./data_balanced/normalization/sciplex_shiftedlog_filt.h5ad</t>
+  </si>
+  <si>
+    <t>./data_balanced/normalization/sciplex_analyticpearson_filt.h5ad</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -395,12 +395,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -417,10 +411,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I129" sqref="I129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,7 +706,7 @@
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
     <col min="3" max="3" width="31.85546875" customWidth="1"/>
     <col min="4" max="4" width="61" customWidth="1"/>
-    <col min="5" max="5" width="53.5703125" customWidth="1"/>
+    <col min="5" max="5" width="76" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -742,16 +735,16 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
@@ -762,16 +755,16 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>11</v>
@@ -782,16 +775,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>11</v>
@@ -802,16 +795,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>11</v>
@@ -822,16 +815,16 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>11</v>
@@ -842,16 +835,16 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>11</v>
@@ -862,16 +855,16 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>11</v>
@@ -882,16 +875,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>11</v>
@@ -902,16 +895,16 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>11</v>
@@ -922,16 +915,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>11</v>
@@ -942,16 +935,16 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>11</v>
@@ -962,16 +955,16 @@
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>11</v>
@@ -982,16 +975,16 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>11</v>
@@ -1002,16 +995,16 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>11</v>
@@ -1022,16 +1015,16 @@
         <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>11</v>
@@ -1042,16 +1035,16 @@
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>11</v>
@@ -1062,16 +1055,16 @@
         <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>11</v>
@@ -1082,16 +1075,16 @@
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>11</v>
@@ -1102,16 +1095,16 @@
         <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>11</v>
@@ -1122,16 +1115,16 @@
         <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>11</v>
@@ -1142,16 +1135,16 @@
         <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>23</v>
+        <v>103</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>11</v>
@@ -1162,16 +1155,16 @@
         <v>8</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>23</v>
+        <v>103</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>11</v>
@@ -1182,16 +1175,16 @@
         <v>7</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>23</v>
+        <v>103</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>11</v>
@@ -1202,16 +1195,16 @@
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>23</v>
+        <v>103</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>11</v>
@@ -1222,16 +1215,16 @@
         <v>10</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>23</v>
+        <v>103</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>11</v>
@@ -1242,16 +1235,16 @@
         <v>9</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>11</v>
@@ -1262,16 +1255,16 @@
         <v>8</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>11</v>
@@ -1282,16 +1275,16 @@
         <v>7</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>11</v>
@@ -1302,16 +1295,16 @@
         <v>6</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>11</v>
@@ -1322,16 +1315,16 @@
         <v>10</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>11</v>
@@ -1342,16 +1335,16 @@
         <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D32" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="E32" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="F32" t="s">
         <v>11</v>
@@ -1362,16 +1355,16 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D33" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="E33" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="F33" t="s">
         <v>11</v>
@@ -1382,16 +1375,16 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C34" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E34" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="F34" t="s">
         <v>11</v>
@@ -1402,16 +1395,16 @@
         <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C35" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D35" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="E35" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="F35" t="s">
         <v>11</v>
@@ -1422,16 +1415,16 @@
         <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C36" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="E36" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="F36" t="s">
         <v>11</v>
@@ -1442,16 +1435,16 @@
         <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C37" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D37" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="E37" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
       <c r="F37" t="s">
         <v>11</v>
@@ -1462,16 +1455,16 @@
         <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C38" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D38" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="E38" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
       <c r="F38" t="s">
         <v>11</v>
@@ -1482,16 +1475,16 @@
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C39" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D39" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="E39" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
       <c r="F39" t="s">
         <v>11</v>
@@ -1502,16 +1495,16 @@
         <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C40" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D40" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="E40" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
       <c r="F40" t="s">
         <v>11</v>
@@ -1522,16 +1515,16 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C41" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D41" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="E41" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
       <c r="F41" t="s">
         <v>11</v>
@@ -1542,16 +1535,16 @@
         <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C42" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D42" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="E42" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="F42" t="s">
         <v>11</v>
@@ -1562,16 +1555,16 @@
         <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C43" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D43" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="E43" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="F43" t="s">
         <v>11</v>
@@ -1582,16 +1575,16 @@
         <v>7</v>
       </c>
       <c r="B44" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C44" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D44" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="E44" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="F44" t="s">
         <v>11</v>
@@ -1602,16 +1595,16 @@
         <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C45" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D45" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="E45" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="F45" t="s">
         <v>11</v>
@@ -1622,16 +1615,16 @@
         <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C46" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D46" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="E46" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="F46" t="s">
         <v>11</v>
@@ -1642,16 +1635,16 @@
         <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C47" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D47" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="E47" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
       <c r="F47" t="s">
         <v>11</v>
@@ -1662,16 +1655,16 @@
         <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C48" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D48" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="E48" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
       <c r="F48" t="s">
         <v>11</v>
@@ -1682,16 +1675,16 @@
         <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C49" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D49" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="E49" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
       <c r="F49" t="s">
         <v>11</v>
@@ -1702,16 +1695,16 @@
         <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C50" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D50" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="E50" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
       <c r="F50" t="s">
         <v>11</v>
@@ -1722,16 +1715,16 @@
         <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C51" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D51" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="E51" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
       <c r="F51" t="s">
         <v>11</v>
@@ -1742,16 +1735,16 @@
         <v>9</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>36</v>
+        <v>109</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>11</v>
@@ -1762,16 +1755,16 @@
         <v>8</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>36</v>
+        <v>109</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>11</v>
@@ -1782,16 +1775,16 @@
         <v>7</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>36</v>
+        <v>109</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>11</v>
@@ -1802,16 +1795,16 @@
         <v>6</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>36</v>
+        <v>109</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>11</v>
@@ -1822,16 +1815,16 @@
         <v>10</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>36</v>
+        <v>109</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>11</v>
@@ -1842,16 +1835,16 @@
         <v>9</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>11</v>
@@ -1862,16 +1855,16 @@
         <v>8</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>11</v>
@@ -1882,16 +1875,16 @@
         <v>7</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>11</v>
@@ -1902,16 +1895,16 @@
         <v>6</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>11</v>
@@ -1922,16 +1915,16 @@
         <v>10</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>11</v>
@@ -1942,16 +1935,16 @@
         <v>9</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>11</v>
@@ -1962,16 +1955,16 @@
         <v>8</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>11</v>
@@ -1982,16 +1975,16 @@
         <v>7</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>11</v>
@@ -2002,16 +1995,16 @@
         <v>6</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>11</v>
@@ -2022,16 +2015,16 @@
         <v>10</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>11</v>
@@ -2042,16 +2035,16 @@
         <v>9</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>11</v>
@@ -2062,16 +2055,16 @@
         <v>8</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>11</v>
@@ -2082,16 +2075,16 @@
         <v>7</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>11</v>
@@ -2102,16 +2095,16 @@
         <v>6</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>11</v>
@@ -2122,16 +2115,16 @@
         <v>10</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D71" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E71" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>11</v>
@@ -2142,19 +2135,19 @@
         <v>9</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="F72" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2162,19 +2155,19 @@
         <v>8</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="F73" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2182,19 +2175,19 @@
         <v>7</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="F74" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2202,19 +2195,19 @@
         <v>6</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="F75" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2222,19 +2215,19 @@
         <v>10</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="F76" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2242,19 +2235,19 @@
         <v>9</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D77" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F77" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2262,19 +2255,19 @@
         <v>8</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D78" s="1" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F78" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2282,19 +2275,19 @@
         <v>7</v>
       </c>
       <c r="B79" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D79" s="1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F79" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2302,19 +2295,19 @@
         <v>6</v>
       </c>
       <c r="B80" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D80" s="1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F80" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2322,19 +2315,19 @@
         <v>10</v>
       </c>
       <c r="B81" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C81" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D81" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F81" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2342,19 +2335,19 @@
         <v>9</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="F82" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2362,19 +2355,19 @@
         <v>8</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="F83" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2382,19 +2375,19 @@
         <v>7</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="F84" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2402,19 +2395,19 @@
         <v>6</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="F85" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2422,19 +2415,19 @@
         <v>10</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="F86" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2442,19 +2435,19 @@
         <v>9</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="F87" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2462,19 +2455,19 @@
         <v>8</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="F88" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2482,19 +2475,19 @@
         <v>7</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="F89" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2502,19 +2495,19 @@
         <v>6</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="F90" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2522,19 +2515,19 @@
         <v>10</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="F91" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2542,19 +2535,19 @@
         <v>9</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>23</v>
+        <v>103</v>
       </c>
       <c r="F92" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -2562,19 +2555,19 @@
         <v>8</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>23</v>
+        <v>103</v>
       </c>
       <c r="F93" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2582,19 +2575,19 @@
         <v>7</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>23</v>
+        <v>103</v>
       </c>
       <c r="F94" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2602,19 +2595,19 @@
         <v>6</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>23</v>
+        <v>103</v>
       </c>
       <c r="F95" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2622,19 +2615,19 @@
         <v>10</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>23</v>
+        <v>103</v>
       </c>
       <c r="F96" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -2642,19 +2635,19 @@
         <v>9</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="F97" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -2662,19 +2655,19 @@
         <v>8</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="F98" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -2682,19 +2675,19 @@
         <v>7</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="F99" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -2702,19 +2695,19 @@
         <v>6</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="F100" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -2722,19 +2715,19 @@
         <v>10</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="F101" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -2742,19 +2735,19 @@
         <v>9</v>
       </c>
       <c r="B102" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C102" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D102" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="E102" t="s">
-        <v>26</v>
-      </c>
-      <c r="F102" s="2">
-        <v>1000</v>
+        <v>105</v>
+      </c>
+      <c r="F102" s="1">
+        <v>10000</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -2762,19 +2755,19 @@
         <v>8</v>
       </c>
       <c r="B103" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C103" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D103" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="E103" t="s">
-        <v>26</v>
-      </c>
-      <c r="F103" s="2">
-        <v>1000</v>
+        <v>105</v>
+      </c>
+      <c r="F103" s="1">
+        <v>10000</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -2782,19 +2775,19 @@
         <v>7</v>
       </c>
       <c r="B104" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C104" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D104" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E104" t="s">
-        <v>26</v>
-      </c>
-      <c r="F104" s="2">
-        <v>1000</v>
+        <v>105</v>
+      </c>
+      <c r="F104" s="1">
+        <v>10000</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -2802,19 +2795,19 @@
         <v>6</v>
       </c>
       <c r="B105" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C105" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D105" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="E105" t="s">
-        <v>26</v>
-      </c>
-      <c r="F105" s="2">
-        <v>1000</v>
+        <v>105</v>
+      </c>
+      <c r="F105" s="1">
+        <v>10000</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -2822,19 +2815,19 @@
         <v>10</v>
       </c>
       <c r="B106" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C106" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D106" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="E106" t="s">
-        <v>26</v>
-      </c>
-      <c r="F106" s="2">
-        <v>1000</v>
+        <v>105</v>
+      </c>
+      <c r="F106" s="1">
+        <v>10000</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -2842,19 +2835,19 @@
         <v>9</v>
       </c>
       <c r="B107" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C107" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D107" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="E107" t="s">
-        <v>28</v>
-      </c>
-      <c r="F107" s="2">
-        <v>1000</v>
+        <v>106</v>
+      </c>
+      <c r="F107" s="1">
+        <v>10000</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -2862,19 +2855,19 @@
         <v>8</v>
       </c>
       <c r="B108" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C108" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D108" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="E108" t="s">
-        <v>28</v>
-      </c>
-      <c r="F108" s="2">
-        <v>1000</v>
+        <v>106</v>
+      </c>
+      <c r="F108" s="1">
+        <v>10000</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -2882,19 +2875,19 @@
         <v>7</v>
       </c>
       <c r="B109" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C109" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D109" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="E109" t="s">
-        <v>28</v>
-      </c>
-      <c r="F109" s="2">
-        <v>1000</v>
+        <v>106</v>
+      </c>
+      <c r="F109" s="1">
+        <v>10000</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -2902,19 +2895,19 @@
         <v>6</v>
       </c>
       <c r="B110" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C110" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D110" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="E110" t="s">
-        <v>28</v>
-      </c>
-      <c r="F110" s="2">
-        <v>1000</v>
+        <v>106</v>
+      </c>
+      <c r="F110" s="1">
+        <v>10000</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -2922,19 +2915,19 @@
         <v>10</v>
       </c>
       <c r="B111" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C111" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D111" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="E111" t="s">
-        <v>28</v>
-      </c>
-      <c r="F111" s="2">
-        <v>1000</v>
+        <v>106</v>
+      </c>
+      <c r="F111" s="1">
+        <v>10000</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -2942,19 +2935,19 @@
         <v>9</v>
       </c>
       <c r="B112" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C112" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D112" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="E112" t="s">
-        <v>31</v>
-      </c>
-      <c r="F112" s="2">
-        <v>1000</v>
+        <v>107</v>
+      </c>
+      <c r="F112" s="1">
+        <v>10000</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -2962,19 +2955,19 @@
         <v>8</v>
       </c>
       <c r="B113" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C113" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D113" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="E113" t="s">
-        <v>31</v>
-      </c>
-      <c r="F113" s="2">
-        <v>1000</v>
+        <v>107</v>
+      </c>
+      <c r="F113" s="1">
+        <v>10000</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -2982,19 +2975,19 @@
         <v>7</v>
       </c>
       <c r="B114" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C114" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D114" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="E114" t="s">
-        <v>31</v>
-      </c>
-      <c r="F114" s="2">
-        <v>1000</v>
+        <v>107</v>
+      </c>
+      <c r="F114" s="1">
+        <v>10000</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3002,19 +2995,19 @@
         <v>6</v>
       </c>
       <c r="B115" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C115" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D115" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="E115" t="s">
-        <v>31</v>
-      </c>
-      <c r="F115" s="2">
-        <v>1000</v>
+        <v>107</v>
+      </c>
+      <c r="F115" s="1">
+        <v>10000</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3022,19 +3015,19 @@
         <v>10</v>
       </c>
       <c r="B116" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C116" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D116" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="E116" t="s">
-        <v>31</v>
-      </c>
-      <c r="F116" s="2">
-        <v>1000</v>
+        <v>107</v>
+      </c>
+      <c r="F116" s="1">
+        <v>10000</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -3042,19 +3035,19 @@
         <v>9</v>
       </c>
       <c r="B117" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C117" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D117" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="E117" t="s">
-        <v>33</v>
-      </c>
-      <c r="F117" s="2">
-        <v>1000</v>
+        <v>108</v>
+      </c>
+      <c r="F117" s="1">
+        <v>10000</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -3062,19 +3055,19 @@
         <v>8</v>
       </c>
       <c r="B118" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C118" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D118" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="E118" t="s">
-        <v>33</v>
-      </c>
-      <c r="F118" s="2">
-        <v>1000</v>
+        <v>108</v>
+      </c>
+      <c r="F118" s="1">
+        <v>10000</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -3082,19 +3075,19 @@
         <v>7</v>
       </c>
       <c r="B119" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C119" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D119" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="E119" t="s">
-        <v>33</v>
-      </c>
-      <c r="F119" s="2">
-        <v>1000</v>
+        <v>108</v>
+      </c>
+      <c r="F119" s="1">
+        <v>10000</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -3102,19 +3095,19 @@
         <v>6</v>
       </c>
       <c r="B120" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C120" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D120" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="E120" t="s">
-        <v>33</v>
-      </c>
-      <c r="F120" s="2">
-        <v>1000</v>
+        <v>108</v>
+      </c>
+      <c r="F120" s="1">
+        <v>10000</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -3122,19 +3115,19 @@
         <v>10</v>
       </c>
       <c r="B121" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C121" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D121" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="E121" t="s">
-        <v>33</v>
-      </c>
-      <c r="F121" s="2">
-        <v>1000</v>
+        <v>108</v>
+      </c>
+      <c r="F121" s="1">
+        <v>10000</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -3142,19 +3135,19 @@
         <v>9</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>36</v>
+        <v>109</v>
       </c>
       <c r="F122" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -3162,19 +3155,19 @@
         <v>8</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>36</v>
+        <v>109</v>
       </c>
       <c r="F123" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -3182,19 +3175,19 @@
         <v>7</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>36</v>
+        <v>109</v>
       </c>
       <c r="F124" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -3202,19 +3195,19 @@
         <v>6</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>36</v>
+        <v>109</v>
       </c>
       <c r="F125" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -3222,19 +3215,19 @@
         <v>10</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>36</v>
+        <v>109</v>
       </c>
       <c r="F126" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -3242,19 +3235,19 @@
         <v>9</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="F127" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -3262,19 +3255,19 @@
         <v>8</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="F128" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -3282,19 +3275,19 @@
         <v>7</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="F129" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
@@ -3302,19 +3295,19 @@
         <v>6</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="F130" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
@@ -3322,19 +3315,19 @@
         <v>10</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="F131" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -3342,19 +3335,19 @@
         <v>9</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="F132" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
@@ -3362,19 +3355,19 @@
         <v>8</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="F133" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
@@ -3382,19 +3375,19 @@
         <v>7</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="F134" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
@@ -3402,19 +3395,19 @@
         <v>6</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="F135" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
@@ -3422,19 +3415,19 @@
         <v>10</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="F136" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
@@ -3442,19 +3435,19 @@
         <v>9</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="F137" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -3462,19 +3455,19 @@
         <v>8</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="F138" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
@@ -3482,19 +3475,19 @@
         <v>7</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="F139" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
@@ -3502,19 +3495,19 @@
         <v>6</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="F140" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
@@ -3522,19 +3515,19 @@
         <v>10</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D141" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E141" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E141" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="F141" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>